<commit_message>
fix df condition statement
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -517,49 +517,49 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1000</v>
+        <v>7.5e-12</v>
       </c>
       <c r="C2" t="n">
-        <v>1000</v>
+        <v>3.3e-10</v>
       </c>
       <c r="D2" t="n">
-        <v>1000</v>
+        <v>7.8e-09</v>
       </c>
       <c r="E2" t="n">
-        <v>1000</v>
+        <v>1.1e-09</v>
       </c>
       <c r="F2" t="n">
-        <v>1000</v>
+        <v>9.799999999999999e-10</v>
       </c>
       <c r="G2" t="n">
-        <v>1000</v>
+        <v>3e-09</v>
       </c>
       <c r="H2" t="n">
-        <v>1000</v>
+        <v>3.4e-09</v>
       </c>
       <c r="I2" t="n">
-        <v>1000</v>
+        <v>4.8e-09</v>
       </c>
       <c r="J2" t="n">
-        <v>1000</v>
+        <v>2.7e-09</v>
       </c>
       <c r="K2" t="n">
-        <v>1000</v>
+        <v>8.599999999999999e-09</v>
       </c>
       <c r="L2" t="n">
-        <v>1000</v>
+        <v>6.2e-09</v>
       </c>
       <c r="M2" t="n">
-        <v>1000</v>
+        <v>3.7e-09</v>
       </c>
       <c r="N2" t="n">
-        <v>1000</v>
+        <v>8.5e-10</v>
       </c>
       <c r="O2" t="n">
-        <v>1000</v>
+        <v>2.4e-09</v>
       </c>
       <c r="P2" t="n">
-        <v>1000</v>
+        <v>5.6e-09</v>
       </c>
     </row>
     <row r="3">
@@ -569,49 +569,49 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1000</v>
+        <v>1.9e-09</v>
       </c>
       <c r="C3" t="n">
-        <v>1000</v>
+        <v>3.6e-09</v>
       </c>
       <c r="D3" t="n">
-        <v>1000</v>
+        <v>7.4e-09</v>
       </c>
       <c r="E3" t="n">
-        <v>1000</v>
+        <v>5.2e-09</v>
       </c>
       <c r="F3" t="n">
-        <v>1000</v>
+        <v>1.1e-09</v>
       </c>
       <c r="G3" t="n">
-        <v>1000</v>
+        <v>3.5e-09</v>
       </c>
       <c r="H3" t="n">
-        <v>1000</v>
+        <v>4.9e-09</v>
       </c>
       <c r="I3" t="n">
-        <v>1000</v>
+        <v>2.4e-09</v>
       </c>
       <c r="J3" t="n">
-        <v>1000</v>
+        <v>9.7e-10</v>
       </c>
       <c r="K3" t="n">
-        <v>1000</v>
+        <v>1.6e-09</v>
       </c>
       <c r="L3" t="n">
-        <v>1000</v>
+        <v>1.7e-09</v>
       </c>
       <c r="M3" t="n">
-        <v>1000</v>
+        <v>4.7e-09</v>
       </c>
       <c r="N3" t="n">
-        <v>1000</v>
+        <v>9e-09</v>
       </c>
       <c r="O3" t="n">
-        <v>1000</v>
+        <v>5.3e-09</v>
       </c>
       <c r="P3" t="n">
-        <v>1000</v>
+        <v>2.9e-09</v>
       </c>
     </row>
     <row r="4">
@@ -621,49 +621,49 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1000</v>
+        <v>6.6e-09</v>
       </c>
       <c r="C4" t="n">
-        <v>1000</v>
+        <v>1.5e-09</v>
       </c>
       <c r="D4" t="n">
-        <v>1000</v>
+        <v>7.9e-10</v>
       </c>
       <c r="E4" t="n">
-        <v>1000</v>
+        <v>3e-09</v>
       </c>
       <c r="F4" t="n">
-        <v>1000</v>
+        <v>4.6e-09</v>
       </c>
       <c r="G4" t="n">
-        <v>1000</v>
+        <v>1.4e-09</v>
       </c>
       <c r="H4" t="n">
-        <v>1000</v>
+        <v>2.7e-09</v>
       </c>
       <c r="I4" t="n">
-        <v>1000</v>
+        <v>2.5e-09</v>
       </c>
       <c r="J4" t="n">
-        <v>1000</v>
+        <v>6.8e-09</v>
       </c>
       <c r="K4" t="n">
-        <v>1000</v>
+        <v>1.2e-09</v>
       </c>
       <c r="L4" t="n">
-        <v>1000</v>
+        <v>5.5e-09</v>
       </c>
       <c r="M4" t="n">
-        <v>1000</v>
+        <v>4.1e-09</v>
       </c>
       <c r="N4" t="n">
-        <v>1000</v>
+        <v>4.9e-09</v>
       </c>
       <c r="O4" t="n">
-        <v>1000</v>
+        <v>6.7e-10</v>
       </c>
       <c r="P4" t="n">
-        <v>1000</v>
+        <v>3.4e-09</v>
       </c>
     </row>
     <row r="5">
@@ -673,49 +673,49 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1000</v>
+        <v>3.6e-09</v>
       </c>
       <c r="C5" t="n">
-        <v>1000</v>
+        <v>1.1e-09</v>
       </c>
       <c r="D5" t="n">
-        <v>1000</v>
+        <v>5.4e-09</v>
       </c>
       <c r="E5" t="n">
-        <v>1000</v>
+        <v>3.7e-09</v>
       </c>
       <c r="F5" t="n">
-        <v>1000</v>
+        <v>1.7e-09</v>
       </c>
       <c r="G5" t="n">
-        <v>1000</v>
+        <v>1e-09</v>
       </c>
       <c r="H5" t="n">
-        <v>1000</v>
+        <v>7.699999999999999e-09</v>
       </c>
       <c r="I5" t="n">
-        <v>1000</v>
+        <v>5.3e-10</v>
       </c>
       <c r="J5" t="n">
-        <v>1000</v>
+        <v>4.9e-09</v>
       </c>
       <c r="K5" t="n">
-        <v>1000</v>
+        <v>1.5e-09</v>
       </c>
       <c r="L5" t="n">
-        <v>1000</v>
+        <v>9.900000000000001e-10</v>
       </c>
       <c r="M5" t="n">
-        <v>1000</v>
+        <v>4e-09</v>
       </c>
       <c r="N5" t="n">
-        <v>1000</v>
+        <v>1.1e-09</v>
       </c>
       <c r="O5" t="n">
-        <v>1000</v>
+        <v>6e-09</v>
       </c>
       <c r="P5" t="n">
-        <v>1000</v>
+        <v>2.1e-09</v>
       </c>
     </row>
     <row r="6">
@@ -725,49 +725,49 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1000</v>
+        <v>1e-08</v>
       </c>
       <c r="C6" t="n">
-        <v>1000</v>
+        <v>1e-08</v>
       </c>
       <c r="D6" t="n">
-        <v>1000</v>
+        <v>1e-08</v>
       </c>
       <c r="E6" t="n">
-        <v>1000</v>
+        <v>1e-08</v>
       </c>
       <c r="F6" t="n">
-        <v>1000</v>
+        <v>1e-08</v>
       </c>
       <c r="G6" t="n">
-        <v>1000</v>
+        <v>1e-08</v>
       </c>
       <c r="H6" t="n">
-        <v>1000</v>
+        <v>1e-08</v>
       </c>
       <c r="I6" t="n">
-        <v>1000</v>
+        <v>1e-08</v>
       </c>
       <c r="J6" t="n">
-        <v>1000</v>
+        <v>1e-08</v>
       </c>
       <c r="K6" t="n">
-        <v>1000</v>
+        <v>1e-08</v>
       </c>
       <c r="L6" t="n">
-        <v>1000</v>
+        <v>1e-08</v>
       </c>
       <c r="M6" t="n">
-        <v>1000</v>
+        <v>1e-08</v>
       </c>
       <c r="N6" t="n">
-        <v>1000</v>
+        <v>1e-08</v>
       </c>
       <c r="O6" t="n">
-        <v>1000</v>
+        <v>1e-08</v>
       </c>
       <c r="P6" t="n">
-        <v>1000</v>
+        <v>1e-08</v>
       </c>
     </row>
     <row r="7">
@@ -777,49 +777,49 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1000</v>
+        <v>2e-09</v>
       </c>
       <c r="C7" t="n">
-        <v>1000</v>
+        <v>2.5e-09</v>
       </c>
       <c r="D7" t="n">
-        <v>1000</v>
+        <v>3.1e-09</v>
       </c>
       <c r="E7" t="n">
-        <v>1000</v>
+        <v>3.8e-09</v>
       </c>
       <c r="F7" t="n">
-        <v>1000</v>
+        <v>4.1e-09</v>
       </c>
       <c r="G7" t="n">
-        <v>1000</v>
+        <v>6.4e-10</v>
       </c>
       <c r="H7" t="n">
-        <v>1000</v>
+        <v>1.8e-09</v>
       </c>
       <c r="I7" t="n">
-        <v>1000</v>
+        <v>4e-09</v>
       </c>
       <c r="J7" t="n">
-        <v>1000</v>
+        <v>1.4e-09</v>
       </c>
       <c r="K7" t="n">
-        <v>1000</v>
+        <v>2.9e-09</v>
       </c>
       <c r="L7" t="n">
-        <v>1000</v>
+        <v>2.2e-09</v>
       </c>
       <c r="M7" t="n">
-        <v>1000</v>
+        <v>4.3e-10</v>
       </c>
       <c r="N7" t="n">
-        <v>1000</v>
+        <v>3.3e-09</v>
       </c>
       <c r="O7" t="n">
-        <v>1000</v>
+        <v>3e-09</v>
       </c>
       <c r="P7" t="n">
-        <v>1000</v>
+        <v>3.4e-09</v>
       </c>
     </row>
     <row r="8">
@@ -829,49 +829,49 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>1000</v>
+        <v>6.4e-09</v>
       </c>
       <c r="C8" t="n">
-        <v>1000</v>
+        <v>4e-09</v>
       </c>
       <c r="D8" t="n">
-        <v>1000</v>
+        <v>7.3e-09</v>
       </c>
       <c r="E8" t="n">
-        <v>1000</v>
+        <v>2.3e-09</v>
       </c>
       <c r="F8" t="n">
-        <v>1000</v>
+        <v>5.8e-09</v>
       </c>
       <c r="G8" t="n">
-        <v>1000</v>
+        <v>4.6e-09</v>
       </c>
       <c r="H8" t="n">
-        <v>1000</v>
+        <v>8.7e-09</v>
       </c>
       <c r="I8" t="n">
-        <v>1000</v>
+        <v>9.4e-09</v>
       </c>
       <c r="J8" t="n">
-        <v>1000</v>
+        <v>4.2e-09</v>
       </c>
       <c r="K8" t="n">
-        <v>1000</v>
+        <v>9.6e-09</v>
       </c>
       <c r="L8" t="n">
-        <v>1000</v>
+        <v>3.4e-09</v>
       </c>
       <c r="M8" t="n">
-        <v>1000</v>
+        <v>4.3e-10</v>
       </c>
       <c r="N8" t="n">
-        <v>1000</v>
+        <v>8.799999999999999e-09</v>
       </c>
       <c r="O8" t="n">
-        <v>1000</v>
+        <v>8.400000000000001e-09</v>
       </c>
       <c r="P8" t="n">
-        <v>1000</v>
+        <v>5.4e-09</v>
       </c>
     </row>
     <row r="9">
@@ -881,49 +881,49 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>1000</v>
+        <v>8.1e-09</v>
       </c>
       <c r="C9" t="n">
-        <v>1000</v>
+        <v>3.3e-09</v>
       </c>
       <c r="D9" t="n">
-        <v>1000</v>
+        <v>9.5e-10</v>
       </c>
       <c r="E9" t="n">
-        <v>1000</v>
+        <v>2.6e-09</v>
       </c>
       <c r="F9" t="n">
-        <v>1000</v>
+        <v>3.1e-09</v>
       </c>
       <c r="G9" t="n">
-        <v>1000</v>
+        <v>5.2e-10</v>
       </c>
       <c r="H9" t="n">
-        <v>1000</v>
+        <v>7.499999999999999e-09</v>
       </c>
       <c r="I9" t="n">
-        <v>1000</v>
+        <v>6.7e-09</v>
       </c>
       <c r="J9" t="n">
-        <v>1000</v>
+        <v>7.3e-09</v>
       </c>
       <c r="K9" t="n">
-        <v>1000</v>
+        <v>1.7e-09</v>
       </c>
       <c r="L9" t="n">
-        <v>1000</v>
+        <v>1.2e-09</v>
       </c>
       <c r="M9" t="n">
-        <v>1000</v>
+        <v>4.5e-09</v>
       </c>
       <c r="N9" t="n">
-        <v>1000</v>
+        <v>2.2e-09</v>
       </c>
       <c r="O9" t="n">
-        <v>1000</v>
+        <v>7.4e-09</v>
       </c>
       <c r="P9" t="n">
-        <v>1000</v>
+        <v>5.9e-10</v>
       </c>
     </row>
     <row r="10">
@@ -933,49 +933,49 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>1000</v>
+        <v>2.3e-09</v>
       </c>
       <c r="C10" t="n">
-        <v>1000</v>
+        <v>5e-09</v>
       </c>
       <c r="D10" t="n">
-        <v>1000</v>
+        <v>3.1e-09</v>
       </c>
       <c r="E10" t="n">
-        <v>1000</v>
+        <v>6.2e-09</v>
       </c>
       <c r="F10" t="n">
-        <v>1000</v>
+        <v>2.5e-09</v>
       </c>
       <c r="G10" t="n">
-        <v>1000</v>
+        <v>3.9e-09</v>
       </c>
       <c r="H10" t="n">
-        <v>1000</v>
+        <v>3e-09</v>
       </c>
       <c r="I10" t="n">
-        <v>1000</v>
+        <v>1.7e-09</v>
       </c>
       <c r="J10" t="n">
-        <v>1000</v>
+        <v>6.7e-09</v>
       </c>
       <c r="K10" t="n">
-        <v>1000</v>
+        <v>1.7e-09</v>
       </c>
       <c r="L10" t="n">
-        <v>1000</v>
+        <v>2.6e-09</v>
       </c>
       <c r="M10" t="n">
-        <v>1000</v>
+        <v>2.8e-09</v>
       </c>
       <c r="N10" t="n">
-        <v>1000</v>
+        <v>1.2e-09</v>
       </c>
       <c r="O10" t="n">
-        <v>1000</v>
+        <v>5.8e-09</v>
       </c>
       <c r="P10" t="n">
-        <v>1000</v>
+        <v>3.2e-10</v>
       </c>
     </row>
     <row r="11">
@@ -985,49 +985,49 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>1000</v>
+        <v>2.7e-09</v>
       </c>
       <c r="C11" t="n">
-        <v>1000</v>
+        <v>3.3e-09</v>
       </c>
       <c r="D11" t="n">
-        <v>1000</v>
+        <v>3.6e-09</v>
       </c>
       <c r="E11" t="n">
-        <v>1000</v>
+        <v>1.4e-09</v>
       </c>
       <c r="F11" t="n">
-        <v>1000</v>
+        <v>3.6e-09</v>
       </c>
       <c r="G11" t="n">
-        <v>1000</v>
+        <v>5.9e-09</v>
       </c>
       <c r="H11" t="n">
-        <v>1000</v>
+        <v>1.3e-09</v>
       </c>
       <c r="I11" t="n">
-        <v>1000</v>
+        <v>1.7e-09</v>
       </c>
       <c r="J11" t="n">
-        <v>1000</v>
+        <v>8.7e-09</v>
       </c>
       <c r="K11" t="n">
-        <v>1000</v>
+        <v>1.5e-09</v>
       </c>
       <c r="L11" t="n">
-        <v>1000</v>
+        <v>3.6e-09</v>
       </c>
       <c r="M11" t="n">
-        <v>1000</v>
+        <v>4e-09</v>
       </c>
       <c r="N11" t="n">
-        <v>1000</v>
+        <v>4.5e-09</v>
       </c>
       <c r="O11" t="n">
-        <v>1000</v>
+        <v>5.7e-09</v>
       </c>
       <c r="P11" t="n">
-        <v>1000</v>
+        <v>2.8e-10</v>
       </c>
     </row>
     <row r="12">
@@ -1037,49 +1037,49 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>1000</v>
+        <v>1.7e-09</v>
       </c>
       <c r="C12" t="n">
-        <v>1000</v>
+        <v>1.3e-09</v>
       </c>
       <c r="D12" t="n">
-        <v>1000</v>
+        <v>2.9e-09</v>
       </c>
       <c r="E12" t="n">
-        <v>1000</v>
+        <v>2.1e-09</v>
       </c>
       <c r="F12" t="n">
-        <v>1000</v>
+        <v>2.4e-09</v>
       </c>
       <c r="G12" t="n">
-        <v>1000</v>
+        <v>1.9e-09</v>
       </c>
       <c r="H12" t="n">
-        <v>1000</v>
+        <v>4.9e-10</v>
       </c>
       <c r="I12" t="n">
-        <v>1000</v>
+        <v>4.9e-09</v>
       </c>
       <c r="J12" t="n">
-        <v>1000</v>
+        <v>7.6e-10</v>
       </c>
       <c r="K12" t="n">
-        <v>1000</v>
+        <v>5.3e-10</v>
       </c>
       <c r="L12" t="n">
-        <v>1000</v>
+        <v>8.1e-09</v>
       </c>
       <c r="M12" t="n">
-        <v>1000</v>
+        <v>2.4e-09</v>
       </c>
       <c r="N12" t="n">
-        <v>1000</v>
+        <v>4.5e-09</v>
       </c>
       <c r="O12" t="n">
-        <v>1000</v>
+        <v>2.9e-09</v>
       </c>
       <c r="P12" t="n">
-        <v>1000</v>
+        <v>6e-09</v>
       </c>
     </row>
     <row r="13">
@@ -1089,49 +1089,49 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>1000</v>
+        <v>2.2e-09</v>
       </c>
       <c r="C13" t="n">
-        <v>1000</v>
+        <v>1.2e-09</v>
       </c>
       <c r="D13" t="n">
-        <v>1000</v>
+        <v>2.9e-09</v>
       </c>
       <c r="E13" t="n">
-        <v>1000</v>
+        <v>1.5e-09</v>
       </c>
       <c r="F13" t="n">
-        <v>1000</v>
+        <v>2.5e-09</v>
       </c>
       <c r="G13" t="n">
-        <v>1000</v>
+        <v>5.8e-09</v>
       </c>
       <c r="H13" t="n">
-        <v>1000</v>
+        <v>5.8e-10</v>
       </c>
       <c r="I13" t="n">
-        <v>1000</v>
+        <v>4.6e-10</v>
       </c>
       <c r="J13" t="n">
-        <v>1000</v>
+        <v>5.3e-09</v>
       </c>
       <c r="K13" t="n">
-        <v>1000</v>
+        <v>2.6e-09</v>
       </c>
       <c r="L13" t="n">
-        <v>1000</v>
+        <v>3.7e-09</v>
       </c>
       <c r="M13" t="n">
-        <v>1000</v>
+        <v>4.6e-09</v>
       </c>
       <c r="N13" t="n">
-        <v>1000</v>
+        <v>1.2e-09</v>
       </c>
       <c r="O13" t="n">
-        <v>1000</v>
+        <v>1.1e-10</v>
       </c>
       <c r="P13" t="n">
-        <v>1000</v>
+        <v>4.7e-10</v>
       </c>
     </row>
     <row r="14">
@@ -1141,49 +1141,49 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>1000</v>
+        <v>1.3e-09</v>
       </c>
       <c r="C14" t="n">
-        <v>1000</v>
+        <v>2.4e-10</v>
       </c>
       <c r="D14" t="n">
-        <v>1000</v>
+        <v>2.6e-09</v>
       </c>
       <c r="E14" t="n">
-        <v>1000</v>
+        <v>1.6e-09</v>
       </c>
       <c r="F14" t="n">
-        <v>1000</v>
+        <v>1.5e-09</v>
       </c>
       <c r="G14" t="n">
-        <v>1000</v>
+        <v>8.5e-10</v>
       </c>
       <c r="H14" t="n">
-        <v>1000</v>
+        <v>1.7e-11</v>
       </c>
       <c r="I14" t="n">
-        <v>1000</v>
+        <v>5.8e-10</v>
       </c>
       <c r="J14" t="n">
-        <v>1000</v>
+        <v>2.2e-09</v>
       </c>
       <c r="K14" t="n">
-        <v>1000</v>
+        <v>3.9e-10</v>
       </c>
       <c r="L14" t="n">
-        <v>1000</v>
+        <v>9.799999999999999e-10</v>
       </c>
       <c r="M14" t="n">
-        <v>1000</v>
+        <v>1.6e-09</v>
       </c>
       <c r="N14" t="n">
-        <v>1000</v>
+        <v>2.3e-10</v>
       </c>
       <c r="O14" t="n">
-        <v>1000</v>
+        <v>3.6e-09</v>
       </c>
       <c r="P14" t="n">
-        <v>1000</v>
+        <v>8.200000000000001e-09</v>
       </c>
     </row>
     <row r="15">
@@ -1193,49 +1193,49 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>1000</v>
+        <v>1.2e-09</v>
       </c>
       <c r="C15" t="n">
-        <v>1000</v>
+        <v>7.1e-09</v>
       </c>
       <c r="D15" t="n">
-        <v>1000</v>
+        <v>6.8e-09</v>
       </c>
       <c r="E15" t="n">
-        <v>1000</v>
+        <v>1.9e-09</v>
       </c>
       <c r="F15" t="n">
-        <v>1000</v>
+        <v>7.2e-10</v>
       </c>
       <c r="G15" t="n">
-        <v>1000</v>
+        <v>1.3e-09</v>
       </c>
       <c r="H15" t="n">
-        <v>1000</v>
+        <v>6.2e-10</v>
       </c>
       <c r="I15" t="n">
-        <v>1000</v>
+        <v>3.4e-09</v>
       </c>
       <c r="J15" t="n">
-        <v>1000</v>
+        <v>1.7e-09</v>
       </c>
       <c r="K15" t="n">
-        <v>1000</v>
+        <v>2.6e-09</v>
       </c>
       <c r="L15" t="n">
-        <v>1000</v>
+        <v>3.6e-09</v>
       </c>
       <c r="M15" t="n">
-        <v>1000</v>
+        <v>3.9e-10</v>
       </c>
       <c r="N15" t="n">
-        <v>1000</v>
+        <v>9.4e-09</v>
       </c>
       <c r="O15" t="n">
-        <v>1000</v>
+        <v>7e-09</v>
       </c>
       <c r="P15" t="n">
-        <v>1000</v>
+        <v>1.8e-09</v>
       </c>
     </row>
     <row r="16">
@@ -1245,49 +1245,49 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>1000</v>
+        <v>2</v>
       </c>
       <c r="C16" t="n">
-        <v>1000</v>
+        <v>2</v>
       </c>
       <c r="D16" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="E16" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="F16" t="n">
-        <v>1000</v>
+        <v>0.0021</v>
       </c>
       <c r="G16" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="H16" t="n">
-        <v>1000</v>
+        <v>0.002</v>
       </c>
       <c r="I16" t="n">
-        <v>1000</v>
+        <v>0.0007</v>
       </c>
       <c r="J16" t="n">
-        <v>1000</v>
+        <v>2</v>
       </c>
       <c r="K16" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="L16" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M16" t="n">
-        <v>1000</v>
+        <v>2</v>
       </c>
       <c r="N16" t="n">
-        <v>1000</v>
+        <v>2</v>
       </c>
       <c r="O16" t="n">
-        <v>1000</v>
+        <v>7.6e-05</v>
       </c>
       <c r="P16" t="n">
-        <v>1000</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17">
@@ -1297,49 +1297,49 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>1000</v>
+        <v>0.0068</v>
       </c>
       <c r="C17" t="n">
-        <v>1000</v>
+        <v>0.01</v>
       </c>
       <c r="D17" t="n">
-        <v>1000</v>
+        <v>0.031</v>
       </c>
       <c r="E17" t="n">
-        <v>1000</v>
+        <v>0.12</v>
       </c>
       <c r="F17" t="n">
-        <v>1000</v>
+        <v>0.078</v>
       </c>
       <c r="G17" t="n">
-        <v>1000</v>
+        <v>0.27</v>
       </c>
       <c r="H17" t="n">
-        <v>1000</v>
+        <v>0.0086</v>
       </c>
       <c r="I17" t="n">
-        <v>1000</v>
+        <v>0.045</v>
       </c>
       <c r="J17" t="n">
-        <v>1000</v>
+        <v>0.011</v>
       </c>
       <c r="K17" t="n">
-        <v>1000</v>
+        <v>0.018</v>
       </c>
       <c r="L17" t="n">
-        <v>1000</v>
+        <v>0.034</v>
       </c>
       <c r="M17" t="n">
-        <v>1000</v>
+        <v>0.37</v>
       </c>
       <c r="N17" t="n">
-        <v>1000</v>
+        <v>0.016</v>
       </c>
       <c r="O17" t="n">
-        <v>1000</v>
+        <v>0.041</v>
       </c>
       <c r="P17" t="n">
-        <v>1000</v>
+        <v>0.015</v>
       </c>
     </row>
     <row r="18">
@@ -1349,49 +1349,49 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>1000</v>
+        <v>2.5e-09</v>
       </c>
       <c r="C18" t="n">
-        <v>1000</v>
+        <v>2.7e-10</v>
       </c>
       <c r="D18" t="n">
-        <v>1000</v>
+        <v>9.3e-10</v>
       </c>
       <c r="E18" t="n">
-        <v>1000</v>
+        <v>4.1e-09</v>
       </c>
       <c r="F18" t="n">
-        <v>1000</v>
+        <v>1.5e-09</v>
       </c>
       <c r="G18" t="n">
-        <v>1000</v>
+        <v>1.5e-10</v>
       </c>
       <c r="H18" t="n">
-        <v>1000</v>
+        <v>4.9e-09</v>
       </c>
       <c r="I18" t="n">
-        <v>1000</v>
+        <v>4.5e-09</v>
       </c>
       <c r="J18" t="n">
-        <v>1000</v>
+        <v>2.2e-09</v>
       </c>
       <c r="K18" t="n">
-        <v>1000</v>
+        <v>2.6e-09</v>
       </c>
       <c r="L18" t="n">
-        <v>1000</v>
+        <v>3e-09</v>
       </c>
       <c r="M18" t="n">
-        <v>1000</v>
+        <v>1.9e-09</v>
       </c>
       <c r="N18" t="n">
-        <v>1000</v>
+        <v>2e-10</v>
       </c>
       <c r="O18" t="n">
-        <v>1000</v>
+        <v>1.9e-09</v>
       </c>
       <c r="P18" t="n">
-        <v>1000</v>
+        <v>1.6e-09</v>
       </c>
     </row>
     <row r="19">
@@ -1401,49 +1401,49 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>1000</v>
+        <v>1.6e-09</v>
       </c>
       <c r="C19" t="n">
-        <v>1000</v>
+        <v>5.7e-09</v>
       </c>
       <c r="D19" t="n">
-        <v>1000</v>
+        <v>0.00031</v>
       </c>
       <c r="E19" t="n">
-        <v>1000</v>
+        <v>3.4e-09</v>
       </c>
       <c r="F19" t="n">
-        <v>1000</v>
+        <v>2.5e-09</v>
       </c>
       <c r="G19" t="n">
-        <v>1000</v>
+        <v>1.3e-09</v>
       </c>
       <c r="H19" t="n">
-        <v>1000</v>
+        <v>7.4e-09</v>
       </c>
       <c r="I19" t="n">
-        <v>1000</v>
+        <v>2.6e-09</v>
       </c>
       <c r="J19" t="n">
-        <v>1000</v>
+        <v>3e-09</v>
       </c>
       <c r="K19" t="n">
-        <v>1000</v>
+        <v>2.6e-09</v>
       </c>
       <c r="L19" t="n">
-        <v>1000</v>
+        <v>5.3e-10</v>
       </c>
       <c r="M19" t="n">
-        <v>1000</v>
+        <v>1.9e-09</v>
       </c>
       <c r="N19" t="n">
-        <v>1000</v>
+        <v>5e-09</v>
       </c>
       <c r="O19" t="n">
-        <v>1000</v>
+        <v>4.7e-09</v>
       </c>
       <c r="P19" t="n">
-        <v>1000</v>
+        <v>1.5e-09</v>
       </c>
     </row>
     <row r="20">
@@ -1453,49 +1453,49 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>1000</v>
+        <v>0.15</v>
       </c>
       <c r="C20" t="n">
-        <v>1000</v>
+        <v>0.08500000000000001</v>
       </c>
       <c r="D20" t="n">
-        <v>1000</v>
+        <v>0.07099999999999999</v>
       </c>
       <c r="E20" t="n">
-        <v>1000</v>
+        <v>0.2</v>
       </c>
       <c r="F20" t="n">
-        <v>1000</v>
+        <v>0.14</v>
       </c>
       <c r="G20" t="n">
-        <v>1000</v>
+        <v>0.081</v>
       </c>
       <c r="H20" t="n">
-        <v>1000</v>
+        <v>0.012</v>
       </c>
       <c r="I20" t="n">
-        <v>1000</v>
+        <v>0.12</v>
       </c>
       <c r="J20" t="n">
-        <v>1000</v>
+        <v>0.21</v>
       </c>
       <c r="K20" t="n">
-        <v>1000</v>
+        <v>0.16</v>
       </c>
       <c r="L20" t="n">
-        <v>1000</v>
+        <v>0.19</v>
       </c>
       <c r="M20" t="n">
-        <v>1000</v>
+        <v>0.13</v>
       </c>
       <c r="N20" t="n">
-        <v>1000</v>
+        <v>0.17</v>
       </c>
       <c r="O20" t="n">
-        <v>1000</v>
+        <v>0.15</v>
       </c>
       <c r="P20" t="n">
-        <v>1000</v>
+        <v>0.19</v>
       </c>
     </row>
     <row r="21">
@@ -1505,49 +1505,49 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>1000</v>
+        <v>2.5e-09</v>
       </c>
       <c r="C21" t="n">
-        <v>1000</v>
+        <v>2.6e-09</v>
       </c>
       <c r="D21" t="n">
-        <v>1000</v>
+        <v>6.9e-10</v>
       </c>
       <c r="E21" t="n">
-        <v>1000</v>
+        <v>4e-09</v>
       </c>
       <c r="F21" t="n">
-        <v>1000</v>
+        <v>2.4e-09</v>
       </c>
       <c r="G21" t="n">
-        <v>1000</v>
+        <v>2.5e-09</v>
       </c>
       <c r="H21" t="n">
-        <v>1000</v>
+        <v>9.6e-10</v>
       </c>
       <c r="I21" t="n">
-        <v>1000</v>
+        <v>2.5e-09</v>
       </c>
       <c r="J21" t="n">
-        <v>1000</v>
+        <v>5.3e-09</v>
       </c>
       <c r="K21" t="n">
-        <v>1000</v>
+        <v>7.7e-10</v>
       </c>
       <c r="L21" t="n">
-        <v>1000</v>
+        <v>4.2e-09</v>
       </c>
       <c r="M21" t="n">
-        <v>1000</v>
+        <v>8.5e-10</v>
       </c>
       <c r="N21" t="n">
-        <v>1000</v>
+        <v>2.1e-09</v>
       </c>
       <c r="O21" t="n">
-        <v>1000</v>
+        <v>6.3e-09</v>
       </c>
       <c r="P21" t="n">
-        <v>1000</v>
+        <v>5.7e-10</v>
       </c>
     </row>
     <row r="22">
@@ -1557,49 +1557,49 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>1000</v>
+        <v>5.8e-09</v>
       </c>
       <c r="C22" t="n">
-        <v>1000</v>
+        <v>9.4e-09</v>
       </c>
       <c r="D22" t="n">
-        <v>1000</v>
+        <v>1.8e-09</v>
       </c>
       <c r="E22" t="n">
-        <v>1000</v>
+        <v>2e-07</v>
       </c>
       <c r="F22" t="n">
-        <v>1000</v>
+        <v>6.4e-09</v>
       </c>
       <c r="G22" t="n">
-        <v>1000</v>
+        <v>6.5e-09</v>
       </c>
       <c r="H22" t="n">
-        <v>1000</v>
+        <v>7.2e-09</v>
       </c>
       <c r="I22" t="n">
-        <v>1000</v>
+        <v>7.8e-09</v>
       </c>
       <c r="J22" t="n">
-        <v>1000</v>
+        <v>0.93</v>
       </c>
       <c r="K22" t="n">
-        <v>1000</v>
+        <v>5.6e-10</v>
       </c>
       <c r="L22" t="n">
-        <v>1000</v>
+        <v>1.5e-09</v>
       </c>
       <c r="M22" t="n">
-        <v>1000</v>
+        <v>6.4e-09</v>
       </c>
       <c r="N22" t="n">
-        <v>1000</v>
+        <v>8.1e-09</v>
       </c>
       <c r="O22" t="n">
-        <v>1000</v>
+        <v>9.6e-10</v>
       </c>
       <c r="P22" t="n">
-        <v>1000</v>
+        <v>4.2e-09</v>
       </c>
     </row>
     <row r="23">
@@ -1609,49 +1609,49 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>1000</v>
+        <v>9e-09</v>
       </c>
       <c r="C23" t="n">
-        <v>1000</v>
+        <v>9.300000000000001e-09</v>
       </c>
       <c r="D23" t="n">
-        <v>1000</v>
+        <v>6.7e-09</v>
       </c>
       <c r="E23" t="n">
-        <v>1000</v>
+        <v>2.7e-06</v>
       </c>
       <c r="F23" t="n">
-        <v>1000</v>
+        <v>6e-09</v>
       </c>
       <c r="G23" t="n">
-        <v>1000</v>
+        <v>7.1e-09</v>
       </c>
       <c r="H23" t="n">
-        <v>1000</v>
+        <v>7e-09</v>
       </c>
       <c r="I23" t="n">
-        <v>1000</v>
+        <v>4e-09</v>
       </c>
       <c r="J23" t="n">
-        <v>1000</v>
+        <v>5e-09</v>
       </c>
       <c r="K23" t="n">
-        <v>1000</v>
+        <v>2.6e-09</v>
       </c>
       <c r="L23" t="n">
-        <v>1000</v>
+        <v>4.3e-09</v>
       </c>
       <c r="M23" t="n">
-        <v>1000</v>
+        <v>2.8e-09</v>
       </c>
       <c r="N23" t="n">
-        <v>1000</v>
+        <v>2.8e-09</v>
       </c>
       <c r="O23" t="n">
-        <v>1000</v>
+        <v>5.5e-09</v>
       </c>
       <c r="P23" t="n">
-        <v>1000</v>
+        <v>2.7e-09</v>
       </c>
     </row>
     <row r="24">
@@ -1661,49 +1661,49 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="C24" t="n">
-        <v>1000</v>
+        <v>0.2</v>
       </c>
       <c r="D24" t="n">
-        <v>1000</v>
+        <v>0.18</v>
       </c>
       <c r="E24" t="n">
-        <v>1000</v>
+        <v>0.4</v>
       </c>
       <c r="F24" t="n">
-        <v>1000</v>
+        <v>3.9e-09</v>
       </c>
       <c r="G24" t="n">
-        <v>1000</v>
+        <v>0.75</v>
       </c>
       <c r="H24" t="n">
-        <v>1000</v>
+        <v>4.4e-09</v>
       </c>
       <c r="I24" t="n">
-        <v>1000</v>
+        <v>0.6</v>
       </c>
       <c r="J24" t="n">
-        <v>1000</v>
+        <v>0.42</v>
       </c>
       <c r="K24" t="n">
-        <v>1000</v>
+        <v>3e-09</v>
       </c>
       <c r="L24" t="n">
-        <v>1000</v>
+        <v>0.42</v>
       </c>
       <c r="M24" t="n">
-        <v>1000</v>
+        <v>0.093</v>
       </c>
       <c r="N24" t="n">
-        <v>1000</v>
+        <v>0.17</v>
       </c>
       <c r="O24" t="n">
-        <v>1000</v>
+        <v>0.93</v>
       </c>
       <c r="P24" t="n">
-        <v>1000</v>
+        <v>0.19</v>
       </c>
     </row>
     <row r="25">
@@ -1713,49 +1713,49 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>1000</v>
+        <v>6</v>
       </c>
       <c r="C25" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="D25" t="n">
-        <v>1000</v>
+        <v>3.3</v>
       </c>
       <c r="E25" t="n">
-        <v>1000</v>
+        <v>0.74</v>
       </c>
       <c r="F25" t="n">
-        <v>1000</v>
+        <v>6.5</v>
       </c>
       <c r="G25" t="n">
-        <v>1000</v>
+        <v>5.3</v>
       </c>
       <c r="H25" t="n">
-        <v>1000</v>
+        <v>6.4</v>
       </c>
       <c r="I25" t="n">
-        <v>1000</v>
+        <v>5.9</v>
       </c>
       <c r="J25" t="n">
-        <v>1000</v>
+        <v>3.8</v>
       </c>
       <c r="K25" t="n">
-        <v>1000</v>
+        <v>1.1</v>
       </c>
       <c r="L25" t="n">
-        <v>1000</v>
+        <v>5.5</v>
       </c>
       <c r="M25" t="n">
-        <v>1000</v>
+        <v>5.4</v>
       </c>
       <c r="N25" t="n">
-        <v>1000</v>
+        <v>5.6</v>
       </c>
       <c r="O25" t="n">
-        <v>1000</v>
+        <v>6</v>
       </c>
       <c r="P25" t="n">
-        <v>1000</v>
+        <v>6.4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>